<commit_message>
add data tables into webapp, update jquery, bootstrap and datatables js scripts version
</commit_message>
<xml_diff>
--- a/data/sra_metadata/SRP199742_SLX15025_GEP00010.xlsx
+++ b/data/sra_metadata/SRP199742_SLX15025_GEP00010.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="21721"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27840" windowHeight="16680" tabRatio="736"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27840" windowHeight="16680" tabRatio="736" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="10" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="458">
   <si>
     <t>description</t>
   </si>
@@ -320,51 +320,6 @@
   </si>
   <si>
     <t>Tab name</t>
-  </si>
-  <si>
-    <t>G11</t>
-  </si>
-  <si>
-    <t>G12</t>
-  </si>
-  <si>
-    <t>H1</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <t>H3</t>
-  </si>
-  <si>
-    <t>H4</t>
-  </si>
-  <si>
-    <t>H5</t>
-  </si>
-  <si>
-    <t>H6</t>
-  </si>
-  <si>
-    <t>H7</t>
-  </si>
-  <si>
-    <t>H8</t>
-  </si>
-  <si>
-    <t>H9</t>
-  </si>
-  <si>
-    <t>H10</t>
-  </si>
-  <si>
-    <t>H11</t>
-  </si>
-  <si>
-    <t>H12</t>
-  </si>
-  <si>
-    <t>plate_01</t>
   </si>
   <si>
     <t>sequencing_dna_source</t>
@@ -5639,7 +5594,7 @@
   </sheetPr>
   <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
@@ -5653,21 +5608,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="32">
       <c r="A1" s="20" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:3" ht="20">
       <c r="A2" s="21" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="22" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
@@ -5696,20 +5651,20 @@
         <v>2</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="B7" s="3" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="B8" s="3" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>80</v>
@@ -5717,7 +5672,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="B9" s="3" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>53</v>
@@ -5725,7 +5680,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="B10" s="3" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>54</v>
@@ -5733,7 +5688,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="B11" s="3" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>55</v>
@@ -5741,7 +5696,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="B12" s="3" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>56</v>
@@ -5750,10 +5705,10 @@
     <row r="13" spans="1:3" ht="15">
       <c r="A13" s="11"/>
       <c r="B13" s="11" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="6" customFormat="1" ht="18" customHeight="1">
@@ -5773,7 +5728,7 @@
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="10" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -5781,7 +5736,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -5789,7 +5744,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -5802,34 +5757,34 @@
     </row>
     <row r="19" spans="1:3">
       <c r="B19" s="3" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="B20" s="3" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="B21" s="3" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="B22" s="3" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -5853,10 +5808,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="B25" s="3" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -5864,7 +5819,7 @@
         <v>4</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -5888,7 +5843,7 @@
         <v>11</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -5896,12 +5851,12 @@
         <v>12</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="B31" s="3" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>65</v>
@@ -5962,7 +5917,7 @@
         <v>10</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15">
@@ -5971,7 +5926,7 @@
         <v>0</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -5987,18 +5942,18 @@
     </row>
     <row r="41" spans="1:3" ht="30">
       <c r="A41" s="1" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="B42" s="3" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -6014,23 +5969,23 @@
         <v>27</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="B45" s="3" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="B46" s="3" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -6038,15 +5993,15 @@
         <v>28</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="B48" s="3" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -6054,7 +6009,7 @@
         <v>20</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -6062,7 +6017,7 @@
         <v>22</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -6070,7 +6025,7 @@
         <v>21</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -6078,7 +6033,7 @@
         <v>25</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -6128,7 +6083,7 @@
         <v>24</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -6136,7 +6091,7 @@
         <v>23</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -6155,23 +6110,23 @@
         <v>51</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="30" customHeight="1">
       <c r="B64" s="3" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="B65" s="3" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -6179,15 +6134,15 @@
         <v>26</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="B67" s="3" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -6214,7 +6169,7 @@
         <v>4</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -6254,34 +6209,34 @@
     </row>
     <row r="75" spans="1:3" ht="30">
       <c r="A75" s="1" t="s">
-        <v>471</v>
+        <v>456</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>472</v>
+        <v>457</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="B76" s="3" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="B77" s="9" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="B78" s="9" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -6321,7 +6276,7 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -6344,36 +6299,36 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="D2" s="2">
         <v>16</v>
@@ -6388,18 +6343,18 @@
         <v>31</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -6414,18 +6369,18 @@
         <v>31</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="D4" s="2">
         <v>4</v>
@@ -6440,7 +6395,7 @@
         <v>32</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -6506,30 +6461,30 @@
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="E2" s="2">
         <v>90</v>
@@ -6538,18 +6493,18 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="E3" s="2">
         <v>100</v>
@@ -6558,18 +6513,18 @@
         <v>21</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="E4" s="2">
         <v>100</v>
@@ -6578,7 +6533,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -6634,7 +6589,7 @@
   <sheetData>
     <row r="1" spans="1:15" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>4</v>
@@ -6652,7 +6607,7 @@
         <v>12</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>13</v>
@@ -6681,13 +6636,13 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="2" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="D2" s="2">
         <v>53704225</v>
@@ -6702,7 +6657,7 @@
         <v>16</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="I2" s="2">
         <v>53704130</v>
@@ -6711,7 +6666,7 @@
         <v>53704148</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="L2" s="19">
         <v>53704291</v>
@@ -6720,18 +6675,18 @@
         <v>53704310</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="2" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="D3" s="2">
         <v>65637008</v>
@@ -6746,7 +6701,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="I3" s="2">
         <v>65637123</v>
@@ -6755,7 +6710,7 @@
         <v>65637142</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="L3" s="2">
         <v>65637077</v>
@@ -6764,18 +6719,18 @@
         <v>65637096</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="2" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="D4" s="2">
         <v>26481627</v>
@@ -6790,7 +6745,7 @@
         <v>4</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="I4" s="2">
         <v>26481482</v>
@@ -6799,7 +6754,7 @@
         <v>26481500</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="L4" s="2">
         <v>26481710</v>
@@ -6808,7 +6763,7 @@
         <v>26481729</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -6874,7 +6829,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:M97"/>
+  <dimension ref="A1:M85"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -6900,7 +6855,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>19</v>
@@ -6912,13 +6867,13 @@
         <v>28</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>20</v>
@@ -6941,32 +6896,32 @@
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1">
       <c r="A2" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I2" s="15"/>
       <c r="J2" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K2" s="15" t="s">
         <v>41</v>
@@ -6980,32 +6935,32 @@
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1">
       <c r="A3" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="E3" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>464</v>
+        <v>449</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I3" s="15"/>
       <c r="J3" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K3" s="15" t="s">
         <v>41</v>
@@ -7019,32 +6974,32 @@
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1">
       <c r="A4" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I4" s="15"/>
       <c r="J4" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K4" s="15" t="s">
         <v>41</v>
@@ -7058,32 +7013,32 @@
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I5" s="15"/>
       <c r="J5" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K5" s="15" t="s">
         <v>41</v>
@@ -7097,32 +7052,32 @@
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I6" s="15"/>
       <c r="J6" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K6" s="15" t="s">
         <v>41</v>
@@ -7136,32 +7091,32 @@
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1">
       <c r="A7" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I7" s="15"/>
       <c r="J7" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K7" s="15" t="s">
         <v>41</v>
@@ -7175,32 +7130,32 @@
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K8" s="15" t="s">
         <v>41</v>
@@ -7214,32 +7169,32 @@
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I9" s="15"/>
       <c r="J9" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K9" s="15" t="s">
         <v>41</v>
@@ -7253,32 +7208,32 @@
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I10" s="15"/>
       <c r="J10" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K10" s="15" t="s">
         <v>41</v>
@@ -7292,32 +7247,32 @@
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1">
       <c r="A11" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I11" s="15"/>
       <c r="J11" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K11" s="15" t="s">
         <v>41</v>
@@ -7331,32 +7286,32 @@
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1">
       <c r="A12" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I12" s="15"/>
       <c r="J12" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K12" s="15" t="s">
         <v>41</v>
@@ -7370,32 +7325,32 @@
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1">
       <c r="A13" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I13" s="15"/>
       <c r="J13" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K13" s="15" t="s">
         <v>41</v>
@@ -7409,32 +7364,32 @@
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1">
       <c r="A14" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I14" s="15"/>
       <c r="J14" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K14" s="15" t="s">
         <v>41</v>
@@ -7448,32 +7403,32 @@
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1">
       <c r="A15" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I15" s="15"/>
       <c r="J15" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K15" s="15" t="s">
         <v>41</v>
@@ -7487,32 +7442,32 @@
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1">
       <c r="A16" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I16" s="15"/>
       <c r="J16" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K16" s="15" t="s">
         <v>41</v>
@@ -7526,32 +7481,32 @@
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1">
       <c r="A17" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I17" s="15"/>
       <c r="J17" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K17" s="15" t="s">
         <v>41</v>
@@ -7565,32 +7520,32 @@
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1">
       <c r="A18" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I18" s="15"/>
       <c r="J18" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K18" s="15" t="s">
         <v>41</v>
@@ -7604,32 +7559,32 @@
     </row>
     <row r="19" spans="1:13" ht="15" customHeight="1">
       <c r="A19" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I19" s="15"/>
       <c r="J19" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K19" s="15" t="s">
         <v>41</v>
@@ -7643,32 +7598,32 @@
     </row>
     <row r="20" spans="1:13" ht="15" customHeight="1">
       <c r="A20" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I20" s="15"/>
       <c r="J20" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K20" s="15" t="s">
         <v>41</v>
@@ -7682,32 +7637,32 @@
     </row>
     <row r="21" spans="1:13" ht="15" customHeight="1">
       <c r="A21" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="E21" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I21" s="15"/>
       <c r="J21" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K21" s="15" t="s">
         <v>41</v>
@@ -7721,32 +7676,32 @@
     </row>
     <row r="22" spans="1:13" ht="15" customHeight="1">
       <c r="A22" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I22" s="15"/>
       <c r="J22" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K22" s="15" t="s">
         <v>41</v>
@@ -7760,32 +7715,32 @@
     </row>
     <row r="23" spans="1:13" ht="15" customHeight="1">
       <c r="A23" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I23" s="15"/>
       <c r="J23" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K23" s="15" t="s">
         <v>41</v>
@@ -7799,32 +7754,32 @@
     </row>
     <row r="24" spans="1:13" ht="15" customHeight="1">
       <c r="A24" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="E24" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I24" s="15"/>
       <c r="J24" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K24" s="15" t="s">
         <v>41</v>
@@ -7838,32 +7793,32 @@
     </row>
     <row r="25" spans="1:13" ht="15" customHeight="1">
       <c r="A25" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="E25" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I25" s="15"/>
       <c r="J25" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K25" s="15" t="s">
         <v>41</v>
@@ -7877,32 +7832,32 @@
     </row>
     <row r="26" spans="1:13" ht="15" customHeight="1">
       <c r="A26" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="E26" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I26" s="15"/>
       <c r="J26" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K26" s="15" t="s">
         <v>41</v>
@@ -7916,32 +7871,32 @@
     </row>
     <row r="27" spans="1:13" ht="15" customHeight="1">
       <c r="A27" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="E27" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I27" s="15"/>
       <c r="J27" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K27" s="15" t="s">
         <v>41</v>
@@ -7955,32 +7910,32 @@
     </row>
     <row r="28" spans="1:13" ht="15" customHeight="1">
       <c r="A28" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="E28" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I28" s="15"/>
       <c r="J28" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K28" s="15" t="s">
         <v>41</v>
@@ -7994,32 +7949,32 @@
     </row>
     <row r="29" spans="1:13" ht="15" customHeight="1">
       <c r="A29" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="E29" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I29" s="15"/>
       <c r="J29" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K29" s="15" t="s">
         <v>41</v>
@@ -8033,32 +7988,32 @@
     </row>
     <row r="30" spans="1:13" ht="15" customHeight="1">
       <c r="A30" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="E30" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I30" s="15"/>
       <c r="J30" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K30" s="15" t="s">
         <v>41</v>
@@ -8072,32 +8027,32 @@
     </row>
     <row r="31" spans="1:13" ht="15" customHeight="1">
       <c r="A31" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="E31" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I31" s="15"/>
       <c r="J31" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K31" s="15" t="s">
         <v>41</v>
@@ -8111,32 +8066,32 @@
     </row>
     <row r="32" spans="1:13" ht="15" customHeight="1">
       <c r="A32" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="E32" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I32" s="15"/>
       <c r="J32" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K32" s="15" t="s">
         <v>41</v>
@@ -8150,32 +8105,32 @@
     </row>
     <row r="33" spans="1:13" ht="15" customHeight="1">
       <c r="A33" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="E33" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I33" s="15"/>
       <c r="J33" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K33" s="15" t="s">
         <v>41</v>
@@ -8189,32 +8144,32 @@
     </row>
     <row r="34" spans="1:13" ht="15" customHeight="1">
       <c r="A34" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="E34" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I34" s="15"/>
       <c r="J34" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K34" s="15" t="s">
         <v>41</v>
@@ -8228,32 +8183,32 @@
     </row>
     <row r="35" spans="1:13" ht="15" customHeight="1">
       <c r="A35" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="E35" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I35" s="15"/>
       <c r="J35" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K35" s="15" t="s">
         <v>41</v>
@@ -8267,32 +8222,32 @@
     </row>
     <row r="36" spans="1:13" ht="15" customHeight="1">
       <c r="A36" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="E36" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I36" s="15"/>
       <c r="J36" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K36" s="15" t="s">
         <v>41</v>
@@ -8306,32 +8261,32 @@
     </row>
     <row r="37" spans="1:13" ht="15" customHeight="1">
       <c r="A37" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
       <c r="E37" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I37" s="15"/>
       <c r="J37" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K37" s="15" t="s">
         <v>41</v>
@@ -8345,32 +8300,32 @@
     </row>
     <row r="38" spans="1:13" ht="15" customHeight="1">
       <c r="A38" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="E38" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I38" s="15"/>
       <c r="J38" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K38" s="15" t="s">
         <v>41</v>
@@ -8384,32 +8339,32 @@
     </row>
     <row r="39" spans="1:13" ht="15" customHeight="1">
       <c r="A39" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="E39" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I39" s="15"/>
       <c r="J39" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K39" s="15" t="s">
         <v>41</v>
@@ -8423,32 +8378,32 @@
     </row>
     <row r="40" spans="1:13" ht="15" customHeight="1">
       <c r="A40" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="E40" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G40" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I40" s="15"/>
       <c r="J40" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K40" s="15" t="s">
         <v>41</v>
@@ -8462,32 +8417,32 @@
     </row>
     <row r="41" spans="1:13" ht="15" customHeight="1">
       <c r="A41" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="E41" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I41" s="15"/>
       <c r="J41" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K41" s="15" t="s">
         <v>41</v>
@@ -8501,32 +8456,32 @@
     </row>
     <row r="42" spans="1:13" ht="15" customHeight="1">
       <c r="A42" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="D42" s="7" t="s">
         <v>307</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>320</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>321</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>322</v>
       </c>
       <c r="E42" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I42" s="15"/>
       <c r="J42" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K42" s="15" t="s">
         <v>41</v>
@@ -8540,32 +8495,32 @@
     </row>
     <row r="43" spans="1:13" ht="15" customHeight="1">
       <c r="A43" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="E43" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I43" s="15"/>
       <c r="J43" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K43" s="15" t="s">
         <v>41</v>
@@ -8579,32 +8534,32 @@
     </row>
     <row r="44" spans="1:13" ht="15" customHeight="1">
       <c r="A44" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="E44" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G44" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I44" s="15"/>
       <c r="J44" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K44" s="15" t="s">
         <v>41</v>
@@ -8618,32 +8573,32 @@
     </row>
     <row r="45" spans="1:13" ht="15" customHeight="1">
       <c r="A45" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="E45" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I45" s="15"/>
       <c r="J45" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K45" s="15" t="s">
         <v>41</v>
@@ -8657,32 +8612,32 @@
     </row>
     <row r="46" spans="1:13" ht="15" customHeight="1">
       <c r="A46" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="E46" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G46" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H46" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I46" s="15"/>
       <c r="J46" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K46" s="15" t="s">
         <v>41</v>
@@ -8696,32 +8651,32 @@
     </row>
     <row r="47" spans="1:13" ht="15" customHeight="1">
       <c r="A47" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="E47" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I47" s="15"/>
       <c r="J47" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K47" s="15" t="s">
         <v>41</v>
@@ -8735,32 +8690,32 @@
     </row>
     <row r="48" spans="1:13" ht="15" customHeight="1">
       <c r="A48" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="E48" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G48" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I48" s="15"/>
       <c r="J48" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K48" s="15" t="s">
         <v>41</v>
@@ -8774,32 +8729,32 @@
     </row>
     <row r="49" spans="1:13" ht="15" customHeight="1">
       <c r="A49" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="E49" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G49" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I49" s="15"/>
       <c r="J49" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K49" s="15" t="s">
         <v>41</v>
@@ -8813,32 +8768,32 @@
     </row>
     <row r="50" spans="1:13" ht="15" customHeight="1">
       <c r="A50" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="E50" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G50" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I50" s="15"/>
       <c r="J50" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K50" s="15" t="s">
         <v>41</v>
@@ -8852,32 +8807,32 @@
     </row>
     <row r="51" spans="1:13" ht="15" customHeight="1">
       <c r="A51" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="E51" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I51" s="15"/>
       <c r="J51" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K51" s="15" t="s">
         <v>41</v>
@@ -8891,32 +8846,32 @@
     </row>
     <row r="52" spans="1:13" ht="15" customHeight="1">
       <c r="A52" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="E52" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G52" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H52" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I52" s="15"/>
       <c r="J52" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K52" s="15" t="s">
         <v>41</v>
@@ -8930,32 +8885,32 @@
     </row>
     <row r="53" spans="1:13" ht="15" customHeight="1">
       <c r="A53" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="E53" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G53" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H53" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I53" s="15"/>
       <c r="J53" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K53" s="15" t="s">
         <v>41</v>
@@ -8969,32 +8924,32 @@
     </row>
     <row r="54" spans="1:13" ht="15" customHeight="1">
       <c r="A54" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="E54" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G54" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H54" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I54" s="15"/>
       <c r="J54" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K54" s="15" t="s">
         <v>41</v>
@@ -9008,32 +8963,32 @@
     </row>
     <row r="55" spans="1:13" ht="15" customHeight="1">
       <c r="A55" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="E55" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G55" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H55" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I55" s="15"/>
       <c r="J55" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K55" s="15" t="s">
         <v>41</v>
@@ -9047,32 +9002,32 @@
     </row>
     <row r="56" spans="1:13" ht="15" customHeight="1">
       <c r="A56" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>364</v>
+        <v>349</v>
       </c>
       <c r="E56" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G56" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H56" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I56" s="15"/>
       <c r="J56" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K56" s="15" t="s">
         <v>41</v>
@@ -9086,32 +9041,32 @@
     </row>
     <row r="57" spans="1:13" ht="15" customHeight="1">
       <c r="A57" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>366</v>
+        <v>351</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
       <c r="E57" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F57" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G57" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H57" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I57" s="15"/>
       <c r="J57" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K57" s="15" t="s">
         <v>41</v>
@@ -9125,32 +9080,32 @@
     </row>
     <row r="58" spans="1:13" ht="15" customHeight="1">
       <c r="A58" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>369</v>
+        <v>354</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="E58" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F58" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G58" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H58" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I58" s="15"/>
       <c r="J58" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K58" s="15" t="s">
         <v>41</v>
@@ -9164,32 +9119,32 @@
     </row>
     <row r="59" spans="1:13" ht="15" customHeight="1">
       <c r="A59" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>372</v>
+        <v>357</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
       <c r="E59" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G59" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H59" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I59" s="15"/>
       <c r="J59" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K59" s="15" t="s">
         <v>41</v>
@@ -9203,32 +9158,32 @@
     </row>
     <row r="60" spans="1:13" ht="15" customHeight="1">
       <c r="A60" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>375</v>
+        <v>360</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>376</v>
+        <v>361</v>
       </c>
       <c r="E60" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F60" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G60" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H60" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I60" s="15"/>
       <c r="J60" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K60" s="15" t="s">
         <v>41</v>
@@ -9242,32 +9197,32 @@
     </row>
     <row r="61" spans="1:13" ht="15" customHeight="1">
       <c r="A61" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>377</v>
+        <v>362</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>378</v>
+        <v>363</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>379</v>
+        <v>364</v>
       </c>
       <c r="E61" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F61" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G61" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H61" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I61" s="15"/>
       <c r="J61" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K61" s="15" t="s">
         <v>41</v>
@@ -9281,32 +9236,32 @@
     </row>
     <row r="62" spans="1:13" ht="15" customHeight="1">
       <c r="A62" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>380</v>
+        <v>365</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="E62" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F62" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G62" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H62" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I62" s="15"/>
       <c r="J62" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K62" s="15" t="s">
         <v>41</v>
@@ -9320,32 +9275,32 @@
     </row>
     <row r="63" spans="1:13" ht="15" customHeight="1">
       <c r="A63" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>384</v>
+        <v>369</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>385</v>
+        <v>370</v>
       </c>
       <c r="E63" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F63" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G63" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H63" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I63" s="15"/>
       <c r="J63" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K63" s="15" t="s">
         <v>41</v>
@@ -9359,32 +9314,32 @@
     </row>
     <row r="64" spans="1:13" ht="15" customHeight="1">
       <c r="A64" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>386</v>
+        <v>371</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>387</v>
+        <v>372</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>388</v>
+        <v>373</v>
       </c>
       <c r="E64" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F64" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G64" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H64" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I64" s="15"/>
       <c r="J64" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K64" s="15" t="s">
         <v>41</v>
@@ -9398,32 +9353,32 @@
     </row>
     <row r="65" spans="1:13" ht="15" customHeight="1">
       <c r="A65" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>389</v>
+        <v>374</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>390</v>
+        <v>375</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>391</v>
+        <v>376</v>
       </c>
       <c r="E65" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F65" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G65" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H65" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I65" s="15"/>
       <c r="J65" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K65" s="15" t="s">
         <v>41</v>
@@ -9437,32 +9392,32 @@
     </row>
     <row r="66" spans="1:13" ht="15" customHeight="1">
       <c r="A66" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>392</v>
+        <v>377</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>393</v>
+        <v>378</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>394</v>
+        <v>379</v>
       </c>
       <c r="E66" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F66" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G66" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H66" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I66" s="15"/>
       <c r="J66" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K66" s="15" t="s">
         <v>41</v>
@@ -9476,32 +9431,32 @@
     </row>
     <row r="67" spans="1:13" ht="15" customHeight="1">
       <c r="A67" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>397</v>
+        <v>382</v>
       </c>
       <c r="E67" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F67" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G67" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H67" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I67" s="15"/>
       <c r="J67" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K67" s="15" t="s">
         <v>41</v>
@@ -9515,32 +9470,32 @@
     </row>
     <row r="68" spans="1:13" ht="15" customHeight="1">
       <c r="A68" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>400</v>
+        <v>385</v>
       </c>
       <c r="E68" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F68" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G68" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H68" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I68" s="15"/>
       <c r="J68" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K68" s="15" t="s">
         <v>41</v>
@@ -9554,32 +9509,32 @@
     </row>
     <row r="69" spans="1:13" ht="15" customHeight="1">
       <c r="A69" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>401</v>
+        <v>386</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>402</v>
+        <v>387</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
       <c r="E69" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F69" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G69" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H69" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I69" s="15"/>
       <c r="J69" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K69" s="15" t="s">
         <v>41</v>
@@ -9593,32 +9548,32 @@
     </row>
     <row r="70" spans="1:13" ht="15" customHeight="1">
       <c r="A70" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>406</v>
+        <v>391</v>
       </c>
       <c r="E70" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F70" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G70" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H70" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I70" s="15"/>
       <c r="J70" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K70" s="15" t="s">
         <v>41</v>
@@ -9632,32 +9587,32 @@
     </row>
     <row r="71" spans="1:13" ht="15" customHeight="1">
       <c r="A71" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>407</v>
+        <v>392</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>408</v>
+        <v>393</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>409</v>
+        <v>394</v>
       </c>
       <c r="E71" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F71" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G71" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H71" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I71" s="15"/>
       <c r="J71" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K71" s="15" t="s">
         <v>41</v>
@@ -9671,32 +9626,32 @@
     </row>
     <row r="72" spans="1:13" ht="15" customHeight="1">
       <c r="A72" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>410</v>
+        <v>395</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>411</v>
+        <v>396</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>412</v>
+        <v>397</v>
       </c>
       <c r="E72" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F72" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G72" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H72" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I72" s="15"/>
       <c r="J72" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K72" s="15" t="s">
         <v>41</v>
@@ -9710,32 +9665,32 @@
     </row>
     <row r="73" spans="1:13" ht="15" customHeight="1">
       <c r="A73" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>413</v>
+        <v>398</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="E73" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F73" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G73" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H73" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I73" s="15"/>
       <c r="J73" s="15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="K73" s="15" t="s">
         <v>41</v>
@@ -9749,32 +9704,32 @@
     </row>
     <row r="74" spans="1:13" ht="15" customHeight="1">
       <c r="A74" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>416</v>
+        <v>401</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="E74" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F74" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G74" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H74" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I74" s="15"/>
       <c r="J74" s="15" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="K74" s="15" t="s">
         <v>41</v>
@@ -9788,32 +9743,32 @@
     </row>
     <row r="75" spans="1:13" ht="15" customHeight="1">
       <c r="A75" s="15" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="E75" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F75" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G75" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H75" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I75" s="15"/>
       <c r="J75" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K75" s="15" t="s">
         <v>41</v>
@@ -9827,32 +9782,32 @@
     </row>
     <row r="76" spans="1:13" ht="15" customHeight="1">
       <c r="A76" s="15" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
       <c r="E76" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F76" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G76" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H76" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I76" s="15"/>
       <c r="J76" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K76" s="15" t="s">
         <v>41</v>
@@ -9866,32 +9821,32 @@
     </row>
     <row r="77" spans="1:13" ht="15" customHeight="1">
       <c r="A77" s="15" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
       <c r="E77" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F77" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G77" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H77" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I77" s="15"/>
       <c r="J77" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K77" s="15" t="s">
         <v>41</v>
@@ -9905,32 +9860,32 @@
     </row>
     <row r="78" spans="1:13" ht="15" customHeight="1">
       <c r="A78" s="15" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="B78" s="15" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
       <c r="E78" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F78" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G78" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H78" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I78" s="15"/>
       <c r="J78" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K78" s="15" t="s">
         <v>41</v>
@@ -9944,32 +9899,32 @@
     </row>
     <row r="79" spans="1:13" ht="15" customHeight="1">
       <c r="A79" s="15" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="B79" s="15" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
       <c r="E79" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F79" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G79" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H79" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I79" s="15"/>
       <c r="J79" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K79" s="15" t="s">
         <v>41</v>
@@ -9983,32 +9938,32 @@
     </row>
     <row r="80" spans="1:13" ht="15" customHeight="1">
       <c r="A80" s="15" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="B80" s="15" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="E80" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F80" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G80" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H80" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I80" s="15"/>
       <c r="J80" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K80" s="15" t="s">
         <v>41</v>
@@ -10022,32 +9977,32 @@
     </row>
     <row r="81" spans="1:13" ht="15" customHeight="1">
       <c r="A81" s="15" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="B81" s="15" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="E81" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F81" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G81" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H81" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I81" s="15"/>
       <c r="J81" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K81" s="15" t="s">
         <v>41</v>
@@ -10061,32 +10016,32 @@
     </row>
     <row r="82" spans="1:13" ht="15" customHeight="1">
       <c r="A82" s="15" t="s">
+        <v>404</v>
+      </c>
+      <c r="B82" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="C82" s="15" t="s">
         <v>419</v>
       </c>
-      <c r="B82" s="15" t="s">
-        <v>283</v>
-      </c>
-      <c r="C82" s="15" t="s">
-        <v>434</v>
-      </c>
       <c r="D82" s="7" t="s">
-        <v>435</v>
+        <v>420</v>
       </c>
       <c r="E82" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F82" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G82" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H82" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I82" s="15"/>
       <c r="J82" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K82" s="15" t="s">
         <v>41</v>
@@ -10100,32 +10055,32 @@
     </row>
     <row r="83" spans="1:13" ht="15" customHeight="1">
       <c r="A83" s="15" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="B83" s="15" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>436</v>
+        <v>421</v>
       </c>
       <c r="D83" s="7" t="s">
-        <v>437</v>
+        <v>422</v>
       </c>
       <c r="E83" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F83" s="15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G83" s="15" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H83" s="15" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I83" s="15"/>
       <c r="J83" s="15" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K83" s="15" t="s">
         <v>41</v>
@@ -10137,118 +10092,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:13">
-      <c r="A84" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" ht="15" customHeight="1">
-      <c r="A85" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13">
-      <c r="A86" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13">
-      <c r="A87" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13">
-      <c r="A88" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13">
-      <c r="A89" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13">
-      <c r="A90" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13">
-      <c r="A91" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13">
-      <c r="A92" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13">
-      <c r="A93" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13">
-      <c r="A94" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13">
-      <c r="A95" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13">
-      <c r="A96" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
+    <row r="85" spans="1:13" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -10289,58 +10133,58 @@
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>438</v>
+        <v>423</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>439</v>
+        <v>424</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>441</v>
+        <v>426</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>442</v>
+        <v>427</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>441</v>
+        <v>426</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>443</v>
+        <v>428</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -10397,7 +10241,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="B2" s="2" t="b">
         <f>TRUE()</f>
@@ -10412,7 +10256,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="B3" s="2" t="b">
         <f>FALSE()</f>
@@ -10427,7 +10271,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
       <c r="B4" s="2" t="b">
         <f>TRUE()</f>
@@ -10442,7 +10286,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
       <c r="B5" s="2" t="b">
         <f>FALSE()</f>
@@ -10457,7 +10301,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
       <c r="B6" s="2" t="b">
         <f>TRUE()</f>
@@ -10472,7 +10316,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
       <c r="B7" s="2" t="b">
         <f>FALSE()</f>
@@ -10487,7 +10331,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="B8" s="2" t="b">
         <f>TRUE()</f>
@@ -10502,7 +10346,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="B9" s="2" t="b">
         <f>FALSE()</f>
@@ -10517,7 +10361,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
       <c r="B10" s="2" t="b">
         <f>TRUE()</f>
@@ -10532,7 +10376,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
       <c r="B11" s="2" t="b">
         <f>FALSE()</f>
@@ -10547,7 +10391,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
       <c r="B12" s="2" t="b">
         <f>TRUE()</f>
@@ -10562,7 +10406,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
       <c r="B13" s="2" t="b">
         <f>FALSE()</f>
@@ -10577,7 +10421,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="B14" s="2" t="b">
         <f>TRUE()</f>
@@ -10592,7 +10436,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="B15" s="2" t="b">
         <f>FALSE()</f>
@@ -10607,7 +10451,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
       <c r="B16" s="2" t="b">
         <f>TRUE()</f>
@@ -10622,7 +10466,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
       <c r="B17" s="2" t="b">
         <f>FALSE()</f>
@@ -10637,7 +10481,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
       <c r="B18" s="2" t="b">
         <f>TRUE()</f>
@@ -10652,7 +10496,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
       <c r="B19" s="2" t="b">
         <f>FALSE()</f>
@@ -10704,145 +10548,145 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="17" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="17" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>447</v>
+        <v>432</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="17" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>448</v>
+        <v>433</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="17" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="17" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>454</v>
+        <v>439</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>465</v>
+        <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>456</v>
+        <v>441</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="7" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>466</v>
+        <v>451</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>457</v>
+        <v>442</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="7" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>458</v>
+        <v>443</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>459</v>
+        <v>444</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="7" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>467</v>
+        <v>452</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>468</v>
+        <v>453</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="17" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>469</v>
+        <v>454</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>460</v>
+        <v>445</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="17" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>470</v>
+        <v>455</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>461</v>
+        <v>446</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="17" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>462</v>
+        <v>447</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>463</v>
+        <v>448</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -10888,7 +10732,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -10897,7 +10741,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>8</v>
@@ -10906,7 +10750,7 @@
         <v>25</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -10946,7 +10790,7 @@
         <v>37</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>29</v>

</xml_diff>